<commit_message>
Added presentations to website
</commit_message>
<xml_diff>
--- a/report/Weekly_Report.xlsx
+++ b/report/Weekly_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ECE554\Capstone Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parid\Documents\GitHub\ECE-554-Capstone-Project\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99052C6B-FAD1-4527-8C65-0193E19EEBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7663B4B1-D03F-497A-9182-5B905EABF69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="2" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Week 0</t>
   </si>
@@ -83,13 +83,22 @@
   </si>
   <si>
     <t>Microarchitechtural Review</t>
+  </si>
+  <si>
+    <t>After we decided that we want to make Just Dance for our project, I read about the different ways to track body movements, image processing algorithms for detecting a body or parts of a body, and algorithms for comparing two videos. At the end of this week we had finalised that we wanted to do DTW for the comparision algorithm.</t>
+  </si>
+  <si>
+    <t>I read about how DTW works, and the different ways to make it faster, and smaller so that it can fit on an FPGA and work in real time. Decided on an implementation we liked.</t>
+  </si>
+  <si>
+    <t>We spent this week deciding our project. Our first idea was a Roomba (automated vaccuum and mop) so I spent this week reading about SLAM before deciding that it is out of the scope of this project for now. Then when we thought about doing Just Dance I read a little about the different ways we would track the dancer (imu vs camera) and how much memory we would need.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,13 +136,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -472,18 +487,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A65ED4-AFC3-7943-A54F-D26BF1B03A96}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -497,7 +512,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -511,7 +526,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -523,12 +538,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -542,7 +557,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -556,7 +571,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -568,7 +583,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -580,12 +595,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -599,7 +614,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -613,7 +628,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -655,14 +670,14 @@
       <selection activeCell="A13" sqref="A13:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,7 +691,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -690,7 +705,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -704,12 +719,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -723,7 +738,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -737,7 +752,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -749,7 +764,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -761,12 +776,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -780,7 +795,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -792,7 +807,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -823,32 +838,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AF9D12-BAE8-1A42-83B7-3859D323A59F}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+    <row r="2" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -860,7 +877,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -872,24 +889,26 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10">
+    <row r="6" spans="1:10" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -901,7 +920,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -913,24 +932,26 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -942,7 +963,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -954,30 +975,20 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A9:J9"/>
+  <mergeCells count="9">
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A13:J13"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -991,14 +1002,14 @@
       <selection sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1010,7 +1021,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1022,7 +1033,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1034,12 +1045,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1051,7 +1062,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1063,7 +1074,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1075,7 +1086,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1087,12 +1098,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1104,7 +1115,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1116,7 +1127,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1153,14 +1164,14 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1172,7 +1183,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1184,7 +1195,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1196,12 +1207,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1213,7 +1224,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1225,7 +1236,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1237,7 +1248,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1249,12 +1260,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1266,7 +1277,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1278,7 +1289,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>

<commit_message>
Gameloop not working yet
</commit_message>
<xml_diff>
--- a/report/Weekly_Report.xlsx
+++ b/report/Weekly_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ECE554\Capstone Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parid\Documents\GitHub\ECE-554-Capstone-Project\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF56B70-54FC-4A17-AEC0-7AD539623D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B993FB0A-B324-4573-B949-CB1CF86CBDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="2" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Week 0</t>
   </si>
@@ -74,13 +74,37 @@
   </si>
   <si>
     <t>Architectural Review</t>
+  </si>
+  <si>
+    <t>We spent this week deciding our project. Our first idea was a Roomba (automated vaccuum and mop) so I spent this week reading about SLAM before deciding that it is out of the scope of this project for now. Then when we thought about doing Just Dance I read a little about the different ways we would track the dancer (imu vs camera) and how much memory we would need.</t>
+  </si>
+  <si>
+    <t>After we decided that we want to make Just Dance for our project, I read about the different ways to track body movements, image processing algorithms for detecting a body or parts of a body, and algorithms for comparing two videos. At the end of this week we had finalised that we wanted to do DTW for the comparision algorithm.</t>
+  </si>
+  <si>
+    <t>I read about how DTW works, and the different ways to make it faster, and smaller so that it can fit on an FPGA and work in real time. Decided on an implementation we liked.</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Implemented and tested a basic DTW and custom shift register. Will need to experiment with types of ditance and minimum units.</t>
+  </si>
+  <si>
+    <t>Weeks 4 and 5</t>
+  </si>
+  <si>
+    <t>While testing DTW further, I realised that the basic version was missing half the functionality. Rewrote a more robust DTW and tested it. The score is much more accurate now.</t>
+  </si>
+  <si>
+    <t>Started working on the game loop.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,13 +142,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -463,18 +490,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A65ED4-AFC3-7943-A54F-D26BF1B03A96}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -488,7 +515,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -500,7 +527,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -512,12 +539,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -531,7 +558,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -543,7 +570,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -555,7 +582,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -567,12 +594,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -586,7 +613,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -598,7 +625,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -635,14 +662,14 @@
       <selection activeCell="A13" sqref="A13:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,7 +683,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -670,7 +697,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -684,12 +711,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -703,7 +730,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,7 +744,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -729,7 +756,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -741,12 +768,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -760,7 +787,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -772,7 +799,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -803,32 +830,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AF9D12-BAE8-1A42-83B7-3859D323A59F}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+    <row r="2" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -840,7 +869,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -852,24 +881,26 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10">
+    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -881,7 +912,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -893,24 +924,26 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="10" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -922,7 +955,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -934,24 +967,36 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A9:J9"/>
+  <mergeCells count="9">
+    <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A13:J13"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
@@ -971,14 +1016,14 @@
       <selection sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -990,7 +1035,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1002,7 +1047,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1014,12 +1059,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1031,7 +1076,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1043,7 +1088,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1055,7 +1100,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1067,12 +1112,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1084,7 +1129,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1096,7 +1141,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1133,14 +1178,14 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1152,7 +1197,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1164,7 +1209,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1176,12 +1221,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1193,7 +1238,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1205,7 +1250,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1217,7 +1262,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1229,12 +1274,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1246,7 +1291,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1258,7 +1303,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>

<commit_message>
Added my weekly reports
</commit_message>
<xml_diff>
--- a/report/Weekly_Report.xlsx
+++ b/report/Weekly_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcjordan3\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B9B86A-D736-456D-9C5A-4C26BB4D963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C67A33-5C2F-418E-A02F-09A7999E7C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Diego" sheetId="4" r:id="rId4"/>
     <sheet name="Shantanu" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +31,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,17 +40,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Week 0</t>
   </si>
   <si>
+    <t>Lightning Talk</t>
+  </si>
+  <si>
     <t>Week 1</t>
   </si>
   <si>
+    <t>Architectural Review</t>
+  </si>
+  <si>
     <t>Week 2</t>
   </si>
   <si>
+    <t>Microarchitectural Review</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Basic Building Blocks Implementation</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Processor/Accelerator Implementation</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Integrating individual modules &amp; testing</t>
+  </si>
+  <si>
+    <t>Week 0 - Lightning Talk</t>
+  </si>
+  <si>
     <t>Introduction Slide</t>
   </si>
   <si>
@@ -58,22 +90,40 @@
     <t>Team Responsibilities</t>
   </si>
   <si>
+    <t>Week 1 - Architectural Review</t>
+  </si>
+  <si>
     <t>Algorithms to Accelerate - DTW</t>
   </si>
   <si>
     <t>Verification of Original Plan</t>
   </si>
   <si>
+    <t>Week 2 - Microarchitectural Review</t>
+  </si>
+  <si>
     <t>Modular-Level Implementation</t>
   </si>
   <si>
-    <t>Lightning Talk</t>
-  </si>
-  <si>
-    <t>Microarchitectural Review</t>
-  </si>
-  <si>
-    <t>Architectural Review</t>
+    <t>Week 3 - Basic Building Blocks Implementation</t>
+  </si>
+  <si>
+    <t>cordic.sv, LUT.sv, counter.sv, cordic_iteration.sv, CORDIC_tb.sv</t>
+  </si>
+  <si>
+    <t>Week 4 - Processor/Accelerator Implementation</t>
+  </si>
+  <si>
+    <t>hier.sv, hier_tb.sv (incomplete)</t>
+  </si>
+  <si>
+    <t>angle_label_unit, angle_label_unit.sv</t>
+  </si>
+  <si>
+    <t>hier.sv, hier_tb.sv</t>
+  </si>
+  <si>
+    <t>Continuing to write tests for the hierarchy</t>
   </si>
   <si>
     <t>We spent this week deciding our project. Our first idea was a Roomba (automated vaccuum and mop) so I spent this week reading about SLAM before deciding that it is out of the scope of this project for now. Then when we thought about doing Just Dance I read a little about the different ways we would track the dancer (imu vs camera) and how much memory we would need.</t>
@@ -85,9 +135,6 @@
     <t>I read about how DTW works, and the different ways to make it faster, and smaller so that it can fit on an FPGA and work in real time. Decided on an implementation we liked.</t>
   </si>
   <si>
-    <t>Week 3</t>
-  </si>
-  <si>
     <t>Implemented and tested a basic DTW and custom shift register. Will need to experiment with types of ditance and minimum units.</t>
   </si>
   <si>
@@ -100,56 +147,71 @@
     <t>Started working on the game loop.</t>
   </si>
   <si>
-    <t>Week 0 - Lightning Talk</t>
-  </si>
-  <si>
-    <t>Week 1 - Architectural Review</t>
-  </si>
-  <si>
-    <t>Week 2 - Microarchitectural Review</t>
-  </si>
-  <si>
-    <t>Week 3 - Basic Building Blocks Implementation</t>
-  </si>
-  <si>
-    <t>cordic.sv, LUT.sv, counter.sv, cordic_iteration.sv, CORDIC_tb.sv</t>
-  </si>
-  <si>
-    <t>Week 4 - Processor/Accelerator Implementation</t>
-  </si>
-  <si>
-    <t>hier.sv, hier_tb.sv (incomplete)</t>
-  </si>
-  <si>
-    <t>angle_label_unit, angle_label_unit.sv</t>
-  </si>
-  <si>
-    <t>Basic Building Blocks Implementation</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Processor/Accelerator Implementation</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>hier.sv, hier_tb.sv</t>
-  </si>
-  <si>
-    <t>Continuing to write tests for the hierarchy</t>
-  </si>
-  <si>
-    <t>Integrating individual modules &amp; testing</t>
+    <t xml:space="preserve">Researched HPS on the DE1-SoC. </t>
+  </si>
+  <si>
+    <t>Tested out and understood the components of the FPGA-HPS Demo program</t>
+  </si>
+  <si>
+    <t>Tried to understand best way to get USB  data onto board processes</t>
+  </si>
+  <si>
+    <t>Decided that it would be easiest to interface with USB via drivers already in linux</t>
+  </si>
+  <si>
+    <t>Began researching linux image onto DE1-SoC - was stalled due to missing wiring (UART - USB)</t>
+  </si>
+  <si>
+    <t>Began understanding how to work with USB through linux</t>
+  </si>
+  <si>
+    <t>Started working on software (c code) to push an image (bitmap) from the usb into the FPGA SDRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debugged code to push an image onto SDRAM of FPGA - got it work. </t>
+  </si>
+  <si>
+    <t>Confirmed that software to push image worked via another software to get the image from FPGA SDRAM and place into USB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebrated very briefly till I looked at the size of 1 bitmap and calculated what the size would be for the entire songs worth of bitmap. </t>
+  </si>
+  <si>
+    <t>Began investigating compression methods that can be applied ahead of time and then decompressed on the board - RLE encoding, using MJPEG, hard coding in the values</t>
+  </si>
+  <si>
+    <t>Did math on potential decompression techniques and made the realization that despite decompression - we would still be over our space limit (we are trying to avoid streaming)</t>
+  </si>
+  <si>
+    <t>Began experimenting with streaming solutions - a double buffer method. Created software to push each image into 2 dedicated addresses in the SDRAM.  Software piece was working. Hardware was not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given timing constraints with Capstone deadline - made the decision that video due to space constraints and streaming complexity,  will be hardcoded in for reference angles. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shifted focus on Audio - began researching the Wolfson Codec and interfacing it with the SPI and SDRAM. Also researched different audio file types. </t>
+  </si>
+  <si>
+    <t>While working through audio module - realized that there might be an uneccesary complexity between synchronizing our audio and video (video plan was to play through PC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Began implementing a way for the video (including the audio) to be stored on my PC, but the play is triggered by the board.  Successfully created software to communicate via COM port. </t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Began the functionality of the video trigger from board.  While trying to run it along side minilab 2 code, ran into an issue of FPGA being re-wired by JTAG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started looking through QSF file and learning more about how the board's programming impacts the hardware components. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -535,20 +597,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A65ED4-AFC3-7943-A54F-D26BF1B03A96}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -560,7 +622,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -572,7 +634,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -584,14 +646,14 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -603,7 +665,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -615,7 +677,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -627,7 +689,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -639,14 +701,14 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -658,7 +720,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -670,7 +732,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -682,34 +744,34 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -733,20 +795,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2032B162-400A-904A-9AB6-0D1C6A289E88}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -758,9 +820,9 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -772,9 +834,9 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -786,14 +848,14 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -805,9 +867,9 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -819,7 +881,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -831,7 +893,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -843,14 +905,14 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -862,7 +924,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -874,9 +936,9 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -888,39 +950,39 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -944,20 +1006,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AF9D12-BAE8-1A42-83B7-3859D323A59F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="49.15" customHeight="1">
+    <row r="2" spans="1:10" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -969,7 +1031,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15.6" customHeight="1">
+    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -981,7 +1043,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15.6" customHeight="1">
+    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -993,14 +1055,14 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="49.15" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1012,7 +1074,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1024,7 +1086,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1036,14 +1098,14 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.15" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1055,7 +1117,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1067,7 +1129,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1079,29 +1141,29 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1125,17 +1187,17 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1147,7 +1209,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1159,7 +1221,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1171,12 +1233,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1188,7 +1250,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1200,7 +1262,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1212,7 +1274,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1224,12 +1286,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1241,7 +1303,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1253,7 +1315,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1284,21 +1346,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E11836-74D5-4176-9C3E-4A3086E8DBFD}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="81.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1309,8 +1376,10 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1321,7 +1390,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1333,13 +1402,15 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1350,8 +1421,10 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1362,7 +1435,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1374,25 +1447,29 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1403,8 +1480,10 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1415,30 +1494,240 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A13:J13"/>
+  <mergeCells count="23">
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A8:J8"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A11:J11"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added evrything to weekly report
</commit_message>
<xml_diff>
--- a/report/Weekly_Report.xlsx
+++ b/report/Weekly_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parid\Documents\GitHub\ECE-554-Capstone-Project\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6614F153-E6B3-4851-A637-903F5D41EDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A8EB0B-44BE-4B31-B457-61C51F43A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{67EA143E-9FE8-7540-9204-94FEFE791C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Week 0</t>
   </si>
@@ -66,18 +66,9 @@
     <t>Basic Building Blocks Implementation</t>
   </si>
   <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Processor/Accelerator Implementation</t>
-  </si>
-  <si>
     <t>Week 5</t>
   </si>
   <si>
-    <t>Integrating individual modules &amp; testing</t>
-  </si>
-  <si>
     <t>Week 0 - Lightning Talk</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>After we decided that we want to make Just Dance for our project, I read about the different ways to track body movements, image processing algorithms for detecting a body or parts of a body, and algorithms for comparing two videos. At the end of this week we had finalised that we wanted to do DTW for the comparision algorithm.</t>
   </si>
   <si>
-    <t>I read about how DTW works, and the different ways to make it faster, and smaller so that it can fit on an FPGA and work in real time. Decided on an implementation we liked.</t>
-  </si>
-  <si>
     <t>Implemented and tested a basic DTW and custom shift register. Will need to experiment with types of ditance and minimum units.</t>
   </si>
   <si>
@@ -235,13 +223,70 @@
   </si>
   <si>
     <t>Worked with team to resolve appropriate color detection</t>
+  </si>
+  <si>
+    <t>I read about how DTW works, and the different ways to make it faster, and smaller so that it can fit on an FPGA and work in real time. Found the following paper that works on a similar FPGA and takes into consideration a Sokoe Chiba band which is used to make the calculation both similar and more accurate.  Paper: M. Hormigo-Jiménez and J. Hormigo, “High-Throughput DTW accelerator with minimum area in AMD FPGA by HLS,” Repositorio Institucional de la Universidad de Málaga, pp. 1–6, Nov. 2023, DOI: 10.1109/dcis58620.2023.10335963.</t>
+  </si>
+  <si>
+    <t>I realised that the paper I was following is overprovisioned for our use and if we allow for a slight error (less that 5%) then we can make the dtw 150x faster and 98.5% smaller. This took a lot of testing in python to make sure that the idea made sense. This DTW was hard to implement as it required a lot of precise timing.</t>
+  </si>
+  <si>
+    <t>We integrated the DTW with Tyler's cordic and I realised that the way I thought the dtw should work is not what Tyler assumed so I made the appropriate changes to dtw, cordic and the tested the two.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We started synthesis testing and there were some problems with how the dtw was written so I fixed that. We merged the code with the peripherals. I wrote a module to isolate colours. Also went to many shops to look for a beanie and gloves </t>
+  </si>
+  <si>
+    <t>Wrote a module to calculate the score from the three DTWs. Worked on isolating the colours which was very difficult and used signal tap for the same. Worked on figuring out why thhe score was taking 1:30 min to turn up.</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduced exposure and bought new gloves for the colour problem. Realised that we were using the wrong fps for the camera which was why the code was taking so long to find the score.  Connecting the uart was stopping the vga from working and smoking the board so I tried to figure that out and realised that the uart was 5V when we needed 3.3V </t>
+  </si>
+  <si>
+    <t>We brainstormed different ideas. We first came up with the idea of making a roomba but on further research we realised that we can't implement SLAM on the FPGA we are using. We instead decided to go with Just Dance and came up with a basic flow of how it would work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We read a lot of papers to decide how to break the logic, and what algorithms to use, Decided on DTW for socring and Cordic for finding angles. We ended up comparing angles as we believe that using angles will make up for the disparities cause by people of different heights and those standing at different distances from the camera. </t>
+  </si>
+  <si>
+    <t>Here we decided the exact breakdown of the modules and how they would interact with each other. We also made a python script to test if the angle logic and dtw actually worked the way we thought they would and make sense for our usecase</t>
+  </si>
+  <si>
+    <t>We broke off individually to work on differentt aspects of the design.</t>
+  </si>
+  <si>
+    <t>Weeks 3-6</t>
+  </si>
+  <si>
+    <t>We integrated the cordic and the angle label unit with the dtw and fixed the integration errors. Tested it all. Towards the end we realised that Diego was MIA and we would need to do his work too so we split that up.</t>
+  </si>
+  <si>
+    <t>Integrated all the modules and tested them. Started synthesis testing and ran everything end to end to see if there were any major integration issues. We also started figuring out how to isolate the colours and went shopping for a beanie and gloves. We couldn't find gloves so we used different coloured papers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We struggled a lot with isolating the colours because the camera isn’t great and with the slightest exposure everything was turning white. We used signal tap to find the colours. Ordered gloves. </t>
+  </si>
+  <si>
+    <t>We also saw that the score was taking 1:30 min to calculate and realised that the bottleneck was the cluster unit. Worked on ways to make it faster. We eventually settled on reducing the number of frames it processes.</t>
+  </si>
+  <si>
+    <t>While trying to spread out the frames we were using we realised that we had the fps of the camera wrong and our original version was correct we just needed to manage the number of frames correctly.</t>
+  </si>
+  <si>
+    <t>We got new TTL serial cables for our UART so that we could have the reference video synchronised with the game but when we plugged in the cable the vga would stop working. We also noticed some smoke. After a lot of debugging we realised that the board needs a 3.3v cable but the one we had is 5v. SInce there are no more cables our final version needs the reference video played manually.</t>
+  </si>
+  <si>
+    <t>Got everything to work just in time for the demo!! (literally)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,6 +296,13 @@
     </font>
     <font>
       <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -279,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -287,10 +339,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -628,20 +684,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A65ED4-AFC3-7943-A54F-D26BF1B03A96}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -655,19 +711,21 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -679,12 +737,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -698,19 +756,21 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -722,7 +782,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -734,12 +794,12 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -753,19 +813,21 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -777,34 +839,74 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -832,16 +934,16 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -853,9 +955,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -867,9 +969,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -881,14 +983,14 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -900,9 +1002,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -914,7 +1016,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -926,7 +1028,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -938,14 +1040,14 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -957,7 +1059,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -969,9 +1071,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -983,39 +1085,39 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1037,34 +1139,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AF9D12-BAE8-1A42-83B7-3859D323A59F}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1076,7 +1181,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1088,26 +1193,26 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1119,7 +1224,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1131,26 +1236,26 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1162,7 +1267,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1174,29 +1279,79 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1223,14 +1378,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1242,7 +1397,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1254,7 +1409,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1266,12 +1421,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1283,7 +1438,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1295,7 +1450,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1307,7 +1462,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1319,12 +1474,12 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1336,7 +1491,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1348,7 +1503,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1381,23 +1536,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E11836-74D5-4176-9C3E-4A3086E8DBFD}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="81.25" customWidth="1"/>
+    <col min="10" max="10" width="81.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1409,9 +1564,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1423,7 +1578,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1435,14 +1590,14 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1454,9 +1609,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1468,7 +1623,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1480,14 +1635,14 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1499,9 +1654,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1513,9 +1668,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1527,9 +1682,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1541,9 +1696,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1555,9 +1710,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1569,9 +1724,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1583,9 +1738,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1597,14 +1752,14 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1616,9 +1771,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1630,9 +1785,9 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1644,9 +1799,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1658,14 +1813,14 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1677,9 +1832,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1691,7 +1846,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1703,14 +1858,14 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1722,9 +1877,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1736,14 +1891,14 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1755,9 +1910,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1769,14 +1924,14 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1788,9 +1943,9 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1802,9 +1957,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1816,7 +1971,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1828,14 +1983,14 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1847,9 +2002,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1863,23 +2018,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A14:J14"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A14:J14"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="A16:J16"/>
     <mergeCell ref="A17:J17"/>
@@ -1890,9 +2042,12 @@
     <mergeCell ref="A32:J32"/>
     <mergeCell ref="A21:J21"/>
     <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A41:J41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>